<commit_message>
removing xlsx files from repo
</commit_message>
<xml_diff>
--- a/bluezones/bzzz.xlsx
+++ b/bluezones/bzzz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smdavis/Code/bee-stuff/bluezones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB20DAB-AB4A-3C45-915F-01B652A71514}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D1A44E-1B20-5949-9CC2-E64FB1A82DD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -268,12 +268,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -308,16 +314,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -637,10 +641,13 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H1" sqref="H1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="10" width="22" style="8"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -658,19 +665,19 @@
       <c r="E1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>72</v>
       </c>
     </row>
@@ -690,7 +697,7 @@
       <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="10">
@@ -713,10 +720,10 @@
       <c r="E3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="F3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="10">
@@ -739,13 +746,13 @@
       <c r="E4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="9">
+      <c r="G4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="10">
         <v>41360</v>
       </c>
       <c r="J4" s="10">
@@ -768,10 +775,10 @@
       <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="F5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J5" s="10">
@@ -794,10 +801,10 @@
       <c r="E6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J6" s="10">
@@ -820,10 +827,10 @@
       <c r="E7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="8" t="s">
+      <c r="F7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="10">
@@ -849,10 +856,10 @@
       <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="8" t="s">
+      <c r="F8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I8" s="10">
@@ -878,10 +885,10 @@
       <c r="E9" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J9" s="10">
@@ -904,10 +911,10 @@
       <c r="E10" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J10" s="10">
@@ -930,10 +937,10 @@
       <c r="E11" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="8" t="s">
+      <c r="F11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J11" s="10">
@@ -956,10 +963,10 @@
       <c r="E12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J12" s="10">
@@ -982,10 +989,10 @@
       <c r="E13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J13" s="10">
@@ -1008,10 +1015,10 @@
       <c r="E14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="F14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J14" s="10">
@@ -1034,10 +1041,10 @@
       <c r="E15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="F15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J15" s="10">
@@ -1060,10 +1067,10 @@
       <c r="E16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J16" s="10">
@@ -1086,10 +1093,10 @@
       <c r="E17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="F17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J17" s="10">
@@ -1112,10 +1119,10 @@
       <c r="E18" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J18" s="10">
@@ -1138,10 +1145,10 @@
       <c r="E19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J19" s="10">
@@ -1164,10 +1171,10 @@
       <c r="E20" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J20" s="10">
@@ -1190,10 +1197,10 @@
       <c r="E21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="8" t="s">
+      <c r="F21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J21" s="10">
@@ -1216,10 +1223,10 @@
       <c r="E22" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J22" s="10">
@@ -1242,10 +1249,10 @@
       <c r="E23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="8" t="s">
+      <c r="F23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J23" s="10">
@@ -1268,10 +1275,10 @@
       <c r="E24" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G24" s="8" t="s">
+      <c r="F24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J24" s="10">
@@ -1294,10 +1301,10 @@
       <c r="E25" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G25" s="8" t="s">
+      <c r="F25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J25" s="10">
@@ -1320,10 +1327,10 @@
       <c r="E26" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="8" t="s">
+      <c r="F26" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J26" s="10">
@@ -1346,10 +1353,10 @@
       <c r="E27" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F27" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J27" s="10">
@@ -1372,10 +1379,10 @@
       <c r="E28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J28" s="10">
@@ -1398,10 +1405,10 @@
       <c r="E29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J29" s="10">
@@ -1424,10 +1431,10 @@
       <c r="E30" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="8" t="s">
+      <c r="F30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J30" s="10">
@@ -1450,10 +1457,10 @@
       <c r="E31" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G31" s="8" t="s">
+      <c r="F31" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J31" s="10">
@@ -1476,10 +1483,10 @@
       <c r="E32" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G32" s="8" t="s">
+      <c r="F32" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J32" s="10">
@@ -1502,10 +1509,10 @@
       <c r="E33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G33" s="8" t="s">
+      <c r="F33" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="9" t="s">
         <v>11</v>
       </c>
       <c r="J33" s="10">
@@ -1528,10 +1535,10 @@
       <c r="E34" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="9" t="s">
         <v>7</v>
       </c>
       <c r="H34" s="10">
@@ -1560,10 +1567,10 @@
       <c r="E35" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="8" t="s">
+      <c r="F35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G35" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J35" s="10">
@@ -1586,10 +1593,10 @@
       <c r="E36" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36" s="8" t="s">
+      <c r="F36" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G36" s="9" t="s">
         <v>11</v>
       </c>
       <c r="J36" s="10">
@@ -1612,10 +1619,10 @@
       <c r="E37" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="8" t="s">
+      <c r="G37" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J37" s="10">
@@ -1638,10 +1645,10 @@
       <c r="E38" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="8" t="s">
+      <c r="F38" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>7</v>
       </c>
       <c r="H38" s="10">
@@ -1667,10 +1674,10 @@
       <c r="E39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F39" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G39" s="8" t="s">
+      <c r="F39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J39" s="10">
@@ -1693,10 +1700,10 @@
       <c r="E40" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G40" s="8" t="s">
+      <c r="F40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J40" s="10">
@@ -1719,10 +1726,10 @@
       <c r="E41" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="8" t="s">
+      <c r="F41" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J41" s="10">
@@ -1745,10 +1752,10 @@
       <c r="E42" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F42" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="8" t="s">
+      <c r="F42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J42" s="10">
@@ -1771,10 +1778,10 @@
       <c r="E43" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F43" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43" s="8" t="s">
+      <c r="F43" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J43" s="10">
@@ -1797,10 +1804,10 @@
       <c r="E44" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G44" s="8" t="s">
+      <c r="F44" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J44" s="10">
@@ -1823,10 +1830,10 @@
       <c r="E45" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G45" s="8" t="s">
+      <c r="G45" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J45" s="10">
@@ -1849,10 +1856,10 @@
       <c r="E46" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G46" s="8" t="s">
+      <c r="F46" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J46" s="10">
@@ -1875,10 +1882,10 @@
       <c r="E47" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G47" s="8" t="s">
+      <c r="F47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J47" s="10">
@@ -1901,10 +1908,10 @@
       <c r="E48" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F48" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G48" s="8" t="s">
+      <c r="F48" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J48" s="10">
@@ -1927,10 +1934,10 @@
       <c r="E49" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F49" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G49" s="8" t="s">
+      <c r="F49" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="9" t="s">
         <v>11</v>
       </c>
       <c r="J49" s="10">
@@ -1953,10 +1960,10 @@
       <c r="E50" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G50" s="8" t="s">
+      <c r="F50" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J50" s="10">
@@ -1979,7 +1986,7 @@
       <c r="E51" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="9" t="s">
         <v>7</v>
       </c>
       <c r="H51" s="10">
@@ -2005,10 +2012,10 @@
       <c r="E52" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G52" s="8" t="s">
+      <c r="F52" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J52" s="10">
@@ -2031,10 +2038,10 @@
       <c r="E53" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G53" s="8" t="s">
+      <c r="G53" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J53" s="10">
@@ -2057,10 +2064,10 @@
       <c r="E54" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F54" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G54" s="8" t="s">
+      <c r="F54" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J54" s="10">
@@ -2083,10 +2090,10 @@
       <c r="E55" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G55" s="8" t="s">
+      <c r="F55" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" s="9" t="s">
         <v>7</v>
       </c>
       <c r="J55" s="10">

</xml_diff>